<commit_message>
Requirements testing and code fixes.
</commit_message>
<xml_diff>
--- a/docs/assignmnet7/Requirments_Matrix.xlsx
+++ b/docs/assignmnet7/Requirments_Matrix.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
   <si>
     <t>Section</t>
   </si>
@@ -243,23 +243,71 @@
     <t>Run will be invoked by 'r' or 'R'. If TM is not running user is prompted for string, by number.  If TM is running the next iteration of transitions will be executed.</t>
   </si>
   <si>
-    <t>Run command will display a message in 2 conditions.  1. Accepted, including # of transitions to discover.  2. Rejected, including # of transitions to discover.</t>
-  </si>
-  <si>
     <t>Quit will be invoked by 'q' or 'Q'.  This will quit any running TM but not exit program.  If not processing string an appropriate message will be displayed.  User is returned to command.</t>
   </si>
   <si>
     <t>Exit will be invoked by 'x' or 'X'. Terminate the application.  If changes were made to input string list output file.  Display message of success or fail to write input string list .str</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Error message displayed</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>empty string was represented as \</t>
+  </si>
+  <si>
+    <t>empty string was ignored.</t>
+  </si>
+  <si>
+    <t>File could not be opened/saved.</t>
+  </si>
+  <si>
+    <t>help is displayed for main menu, but not individual commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run command will display a message in 3 conditions.  1. Accepted, including # of transitions to discover.  2. Rejected, including # of transitions to discover. 3. Instantaneous description </t>
+  </si>
+  <si>
+    <t>exitting is hard</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Regression Result</t>
+  </si>
+  <si>
+    <t>Help added to List function and removed from being displayed at main menu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,7 +466,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -453,7 +500,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -629,14 +675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -644,9 +690,12 @@
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -665,8 +714,23 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>4.0999999999999996</v>
       </c>
@@ -679,8 +743,11 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="5">
         <v>4.0999999999999996</v>
       </c>
@@ -693,8 +760,11 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="5">
         <v>4.0999999999999996</v>
       </c>
@@ -707,8 +777,11 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="5">
         <v>4.0999999999999996</v>
       </c>
@@ -721,8 +794,11 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="5">
         <v>4.0999999999999996</v>
       </c>
@@ -735,8 +811,11 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="5">
         <v>4.2</v>
       </c>
@@ -749,8 +828,11 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="5">
         <v>4.2</v>
       </c>
@@ -763,8 +845,11 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="5">
         <v>4.2</v>
       </c>
@@ -777,8 +862,11 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="5">
         <v>4.2</v>
       </c>
@@ -791,8 +879,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="5">
         <v>4.2</v>
       </c>
@@ -805,8 +896,11 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="5">
         <v>4.2</v>
       </c>
@@ -819,8 +913,11 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="5">
         <v>4.2</v>
       </c>
@@ -833,8 +930,11 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="5">
         <v>4.2</v>
       </c>
@@ -847,8 +947,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="5">
         <v>4.2</v>
       </c>
@@ -861,8 +964,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="5">
         <v>4.2</v>
       </c>
@@ -875,8 +981,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="5">
         <v>4.2</v>
       </c>
@@ -889,8 +998,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="75">
       <c r="A18" s="5">
         <v>4.2</v>
       </c>
@@ -903,8 +1015,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="45">
       <c r="A19" s="5">
         <v>4.2</v>
       </c>
@@ -917,8 +1032,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="5">
         <v>4.2</v>
       </c>
@@ -931,8 +1049,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75">
       <c r="A21" s="5">
         <v>4.2</v>
       </c>
@@ -945,8 +1066,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="5">
         <v>4.2</v>
       </c>
@@ -959,8 +1083,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45">
       <c r="A23" s="5">
         <v>4.2</v>
       </c>
@@ -973,8 +1100,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="5">
         <v>4.3</v>
       </c>
@@ -987,8 +1117,17 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30">
       <c r="A25" s="5">
         <v>4.3</v>
       </c>
@@ -1001,8 +1140,14 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30">
       <c r="A26" s="5">
         <v>4.3</v>
       </c>
@@ -1015,8 +1160,23 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" t="s">
+        <v>85</v>
+      </c>
+      <c r="J26" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30">
       <c r="A27" s="5">
         <v>4.3</v>
       </c>
@@ -1029,8 +1189,23 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27" t="s">
+        <v>86</v>
+      </c>
+      <c r="J27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="5">
         <v>4.3</v>
       </c>
@@ -1043,8 +1218,14 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
       <c r="A29" s="5">
         <v>4.3</v>
       </c>
@@ -1057,8 +1238,14 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
       <c r="A30" s="5">
         <v>4.3</v>
       </c>
@@ -1071,8 +1258,20 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30" t="s">
+        <v>78</v>
+      </c>
+      <c r="K30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30">
       <c r="A31" s="5">
         <v>4.3</v>
       </c>
@@ -1085,8 +1284,20 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>84</v>
+      </c>
+      <c r="J31" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45">
       <c r="A32" s="5">
         <v>4.3</v>
       </c>
@@ -1099,8 +1310,14 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="60">
       <c r="A33" s="5">
         <v>4.3</v>
       </c>
@@ -1113,8 +1330,23 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>84</v>
+      </c>
+      <c r="I33" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="45">
       <c r="A34" s="5">
         <v>5</v>
       </c>
@@ -1127,8 +1359,11 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30">
       <c r="A35" s="8" t="s">
         <v>30</v>
       </c>
@@ -1141,8 +1376,11 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30">
       <c r="A36" s="8" t="s">
         <v>30</v>
       </c>
@@ -1155,8 +1393,14 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="8" t="s">
         <v>30</v>
       </c>
@@ -1169,8 +1413,14 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
         <v>30</v>
       </c>
@@ -1183,8 +1433,14 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="8" t="s">
         <v>30</v>
       </c>
@@ -1197,8 +1453,14 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="45">
       <c r="A40" s="8" t="s">
         <v>30</v>
       </c>
@@ -1211,8 +1473,14 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30">
       <c r="A41" s="5">
         <v>5.2</v>
       </c>
@@ -1225,8 +1493,14 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="H41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="45">
       <c r="A42" s="6">
         <v>5.2</v>
       </c>
@@ -1239,8 +1513,14 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30">
       <c r="A43" s="8" t="s">
         <v>34</v>
       </c>
@@ -1253,8 +1533,14 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>9</v>
+      </c>
+      <c r="H43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="45">
       <c r="A44" s="8" t="s">
         <v>34</v>
       </c>
@@ -1267,8 +1553,26 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>10</v>
+      </c>
+      <c r="H44" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" t="s">
+        <v>88</v>
+      </c>
+      <c r="J44" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" t="s">
+        <v>81</v>
+      </c>
+      <c r="L44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="60">
       <c r="A45" s="8" t="s">
         <v>35</v>
       </c>
@@ -1281,8 +1585,14 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45">
       <c r="A46" s="8" t="s">
         <v>35</v>
       </c>
@@ -1295,8 +1605,14 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30">
       <c r="A47" s="8" t="s">
         <v>37</v>
       </c>
@@ -1309,8 +1625,14 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>13</v>
+      </c>
+      <c r="H47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="8" t="s">
         <v>41</v>
       </c>
@@ -1323,8 +1645,14 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>14</v>
+      </c>
+      <c r="H48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="45">
       <c r="A49" s="8" t="s">
         <v>41</v>
       </c>
@@ -1337,8 +1665,14 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G49" s="2">
+        <v>15</v>
+      </c>
+      <c r="H49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30">
       <c r="A50" s="8" t="s">
         <v>41</v>
       </c>
@@ -1351,8 +1685,14 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>16</v>
+      </c>
+      <c r="H50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="30">
       <c r="A51" s="8" t="s">
         <v>42</v>
       </c>
@@ -1365,8 +1705,14 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>17</v>
+      </c>
+      <c r="H51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="45">
       <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
@@ -1379,8 +1725,14 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>18</v>
+      </c>
+      <c r="H52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="30">
       <c r="A53" s="8" t="s">
         <v>43</v>
       </c>
@@ -1393,8 +1745,14 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>19</v>
+      </c>
+      <c r="H53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="45">
       <c r="A54" s="8" t="s">
         <v>43</v>
       </c>
@@ -1407,8 +1765,14 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>20</v>
+      </c>
+      <c r="H54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="45">
       <c r="A55" s="8" t="s">
         <v>51</v>
       </c>
@@ -1421,8 +1785,14 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>21</v>
+      </c>
+      <c r="H55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="30">
       <c r="A56" s="8" t="s">
         <v>51</v>
       </c>
@@ -1435,8 +1805,14 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>22</v>
+      </c>
+      <c r="H56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="45">
       <c r="A57" s="8" t="s">
         <v>51</v>
       </c>
@@ -1449,8 +1825,14 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>23</v>
+      </c>
+      <c r="H57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="45">
       <c r="A58" s="8" t="s">
         <v>52</v>
       </c>
@@ -1463,8 +1845,14 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>24</v>
+      </c>
+      <c r="H58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="30">
       <c r="A59" s="8" t="s">
         <v>52</v>
       </c>
@@ -1477,8 +1865,14 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>25</v>
+      </c>
+      <c r="H59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="60">
       <c r="A60" s="8" t="s">
         <v>54</v>
       </c>
@@ -1491,8 +1885,14 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
-    </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>26</v>
+      </c>
+      <c r="H60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="75">
       <c r="A61" s="8" t="s">
         <v>54</v>
       </c>
@@ -1500,13 +1900,19 @@
         <v>60</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>27</v>
+      </c>
+      <c r="H61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="60">
       <c r="A62" s="8" t="s">
         <v>55</v>
       </c>
@@ -1514,13 +1920,19 @@
         <v>61</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>28</v>
+      </c>
+      <c r="H62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="60">
       <c r="A63" s="6">
         <v>5.3</v>
       </c>
@@ -1528,11 +1940,26 @@
         <v>62</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
+      <c r="G63">
+        <v>29</v>
+      </c>
+      <c r="H63" t="s">
+        <v>84</v>
+      </c>
+      <c r="I63" t="s">
+        <v>90</v>
+      </c>
+      <c r="J63" t="s">
+        <v>78</v>
+      </c>
+      <c r="K63" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1541,24 +1968,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Regression test results added.
</commit_message>
<xml_diff>
--- a/docs/assignmnet7/Requirments_Matrix.xlsx
+++ b/docs/assignmnet7/Requirments_Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
   <si>
     <t>Section</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>Help added to List function and removed from being displayed at main menu.</t>
+  </si>
+  <si>
+    <t>Note: Run command will not run on '\' as input string</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -679,7 +685,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -985,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="5">
         <v>4.2</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75">
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="5">
         <v>4.2</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45">
+    <row r="19" spans="1:12" ht="45">
       <c r="A19" s="5">
         <v>4.2</v>
       </c>
@@ -1036,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45">
+    <row r="20" spans="1:12" ht="45">
       <c r="A20" s="5">
         <v>4.2</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="75">
+    <row r="21" spans="1:12" ht="75">
       <c r="A21" s="5">
         <v>4.2</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30">
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" s="5">
         <v>4.2</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="45">
+    <row r="23" spans="1:12" ht="45">
       <c r="A23" s="5">
         <v>4.2</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30">
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="5">
         <v>4.3</v>
       </c>
@@ -1126,8 +1132,14 @@
       <c r="I24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="30">
+      <c r="J24" t="s">
+        <v>95</v>
+      </c>
+      <c r="K24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="5">
         <v>4.3</v>
       </c>
@@ -1146,8 +1158,14 @@
       <c r="H25" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="30">
+      <c r="J25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30">
       <c r="A26" s="5">
         <v>4.3</v>
       </c>
@@ -1176,7 +1194,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30">
+    <row r="27" spans="1:12" ht="30">
       <c r="A27" s="5">
         <v>4.3</v>
       </c>
@@ -1204,8 +1222,11 @@
       <c r="K27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+      <c r="L27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30">
       <c r="A28" s="5">
         <v>4.3</v>
       </c>
@@ -1224,8 +1245,14 @@
       <c r="H28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
+      <c r="J28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" s="5">
         <v>4.3</v>
       </c>
@@ -1244,8 +1271,14 @@
       <c r="H29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
+      <c r="J29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30">
       <c r="A30" s="5">
         <v>4.3</v>
       </c>
@@ -1271,7 +1304,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30">
+    <row r="31" spans="1:12" ht="30">
       <c r="A31" s="5">
         <v>4.3</v>
       </c>
@@ -1297,7 +1330,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="45">
+    <row r="32" spans="1:12" ht="45">
       <c r="A32" s="5">
         <v>4.3</v>
       </c>
@@ -1316,6 +1349,12 @@
       <c r="H32" t="s">
         <v>81</v>
       </c>
+      <c r="J32" t="s">
+        <v>95</v>
+      </c>
+      <c r="K32" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="60">
       <c r="A33" s="5">
@@ -1399,6 +1438,12 @@
       <c r="H36" t="s">
         <v>81</v>
       </c>
+      <c r="J36" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="30">
       <c r="A37" s="8" t="s">
@@ -1419,6 +1464,12 @@
       <c r="H37" t="s">
         <v>81</v>
       </c>
+      <c r="J37" t="s">
+        <v>95</v>
+      </c>
+      <c r="K37" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
@@ -1439,6 +1490,12 @@
       <c r="H38" t="s">
         <v>81</v>
       </c>
+      <c r="J38" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="8" t="s">
@@ -1457,6 +1514,12 @@
         <v>1</v>
       </c>
       <c r="H39" t="s">
+        <v>81</v>
+      </c>
+      <c r="J39" t="s">
+        <v>95</v>
+      </c>
+      <c r="K39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1479,6 +1542,12 @@
       <c r="H40" t="s">
         <v>80</v>
       </c>
+      <c r="J40" t="s">
+        <v>95</v>
+      </c>
+      <c r="K40" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="5">
@@ -1499,6 +1568,12 @@
       <c r="H41" t="s">
         <v>81</v>
       </c>
+      <c r="J41" t="s">
+        <v>95</v>
+      </c>
+      <c r="K41" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="45">
       <c r="A42" s="6">
@@ -1519,6 +1594,12 @@
       <c r="H42" t="s">
         <v>81</v>
       </c>
+      <c r="J42" t="s">
+        <v>95</v>
+      </c>
+      <c r="K42" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="8" t="s">
@@ -1539,6 +1620,12 @@
       <c r="H43" t="s">
         <v>81</v>
       </c>
+      <c r="J43" t="s">
+        <v>95</v>
+      </c>
+      <c r="K43" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="45">
       <c r="A44" s="8" t="s">
@@ -1591,6 +1678,12 @@
       <c r="H45" t="s">
         <v>81</v>
       </c>
+      <c r="J45" t="s">
+        <v>95</v>
+      </c>
+      <c r="K45" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="45">
       <c r="A46" s="8" t="s">
@@ -1611,6 +1704,12 @@
       <c r="H46" t="s">
         <v>81</v>
       </c>
+      <c r="J46" t="s">
+        <v>95</v>
+      </c>
+      <c r="K46" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="30">
       <c r="A47" s="8" t="s">
@@ -1631,6 +1730,12 @@
       <c r="H47" t="s">
         <v>81</v>
       </c>
+      <c r="J47" t="s">
+        <v>95</v>
+      </c>
+      <c r="K47" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="8" t="s">
@@ -1651,6 +1756,12 @@
       <c r="H48" t="s">
         <v>81</v>
       </c>
+      <c r="J48" t="s">
+        <v>95</v>
+      </c>
+      <c r="K48" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="45">
       <c r="A49" s="8" t="s">
@@ -1671,6 +1782,12 @@
       <c r="H49" t="s">
         <v>81</v>
       </c>
+      <c r="J49" t="s">
+        <v>95</v>
+      </c>
+      <c r="K49" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" s="8" t="s">
@@ -1691,6 +1808,12 @@
       <c r="H50" t="s">
         <v>81</v>
       </c>
+      <c r="J50" t="s">
+        <v>95</v>
+      </c>
+      <c r="K50" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="8" t="s">
@@ -1711,6 +1834,12 @@
       <c r="H51" t="s">
         <v>81</v>
       </c>
+      <c r="J51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K51" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="52" spans="1:11" ht="45">
       <c r="A52" s="8" t="s">
@@ -1731,6 +1860,12 @@
       <c r="H52" t="s">
         <v>81</v>
       </c>
+      <c r="J52" t="s">
+        <v>95</v>
+      </c>
+      <c r="K52" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="53" spans="1:11" ht="30">
       <c r="A53" s="8" t="s">
@@ -1751,6 +1886,12 @@
       <c r="H53" t="s">
         <v>81</v>
       </c>
+      <c r="J53" t="s">
+        <v>95</v>
+      </c>
+      <c r="K53" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="45">
       <c r="A54" s="8" t="s">
@@ -1771,6 +1912,12 @@
       <c r="H54" t="s">
         <v>81</v>
       </c>
+      <c r="J54" t="s">
+        <v>95</v>
+      </c>
+      <c r="K54" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="45">
       <c r="A55" s="8" t="s">
@@ -1791,6 +1938,12 @@
       <c r="H55" t="s">
         <v>81</v>
       </c>
+      <c r="J55" t="s">
+        <v>95</v>
+      </c>
+      <c r="K55" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="56" spans="1:11" ht="30">
       <c r="A56" s="8" t="s">
@@ -1811,6 +1964,12 @@
       <c r="H56" t="s">
         <v>81</v>
       </c>
+      <c r="J56" t="s">
+        <v>95</v>
+      </c>
+      <c r="K56" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="45">
       <c r="A57" s="8" t="s">
@@ -1831,6 +1990,12 @@
       <c r="H57" t="s">
         <v>81</v>
       </c>
+      <c r="J57" t="s">
+        <v>95</v>
+      </c>
+      <c r="K57" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="58" spans="1:11" ht="45">
       <c r="A58" s="8" t="s">
@@ -1851,6 +2016,12 @@
       <c r="H58" t="s">
         <v>81</v>
       </c>
+      <c r="J58" t="s">
+        <v>95</v>
+      </c>
+      <c r="K58" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="59" spans="1:11" ht="30">
       <c r="A59" s="8" t="s">
@@ -1871,6 +2042,12 @@
       <c r="H59" t="s">
         <v>81</v>
       </c>
+      <c r="J59" t="s">
+        <v>95</v>
+      </c>
+      <c r="K59" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="60">
       <c r="A60" s="8" t="s">
@@ -1891,6 +2068,12 @@
       <c r="H60" t="s">
         <v>81</v>
       </c>
+      <c r="J60" t="s">
+        <v>95</v>
+      </c>
+      <c r="K60" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="61" spans="1:11" ht="75">
       <c r="A61" s="8" t="s">
@@ -1911,6 +2094,12 @@
       <c r="H61" t="s">
         <v>81</v>
       </c>
+      <c r="J61" t="s">
+        <v>95</v>
+      </c>
+      <c r="K61" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="60">
       <c r="A62" s="8" t="s">
@@ -1929,6 +2118,12 @@
         <v>28</v>
       </c>
       <c r="H62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62" t="s">
+        <v>95</v>
+      </c>
+      <c r="K62" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed Test Case 1 description
</commit_message>
<xml_diff>
--- a/docs/assignmnet7/Requirments_Matrix.xlsx
+++ b/docs/assignmnet7/Requirments_Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="107">
   <si>
     <t>Operate as a console application</t>
   </si>
@@ -243,9 +243,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>Error message displayed</t>
-  </si>
-  <si>
     <t>fail</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>Error now displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Bugzilla</t>
   </si>
   <si>
@@ -337,6 +331,12 @@
   </si>
   <si>
     <t>http://cpts442.tricity.wsu.edu/bugzilla/show_bug.cgi?id=59</t>
+  </si>
+  <si>
+    <t>File now saves correctly</t>
+  </si>
+  <si>
+    <t>Blank line is now ignored</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,34 +776,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>94</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>73</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -819,11 +819,17 @@
       <c r="D2" s="13">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="13"/>
+      <c r="H2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -839,11 +845,17 @@
       <c r="D3" s="13">
         <v>1</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="13"/>
+      <c r="H3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -859,11 +871,17 @@
       <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="13"/>
+      <c r="H4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -879,11 +897,17 @@
       <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="13"/>
+      <c r="H5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -899,11 +923,17 @@
       <c r="D6" s="13">
         <v>1</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="13"/>
+      <c r="H6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -919,11 +949,17 @@
       <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="13"/>
+      <c r="H7" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -939,11 +975,17 @@
       <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="13"/>
+      <c r="H8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -959,11 +1001,17 @@
       <c r="D9" s="13">
         <v>1</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="13"/>
+      <c r="H9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -979,11 +1027,17 @@
       <c r="D10" s="13">
         <v>1</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="13"/>
+      <c r="H10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -999,11 +1053,17 @@
       <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1019,11 +1079,17 @@
       <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1039,11 +1105,17 @@
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1059,11 +1131,17 @@
       <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1079,11 +1157,17 @@
       <c r="D15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="13"/>
+      <c r="H15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1099,11 +1183,17 @@
       <c r="D16" s="13">
         <v>1</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1119,11 +1209,17 @@
       <c r="D17" s="13">
         <v>1</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="13"/>
+      <c r="H17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1139,11 +1235,17 @@
       <c r="D18" s="13">
         <v>1</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="13"/>
+      <c r="H18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1159,11 +1261,17 @@
       <c r="D19" s="13">
         <v>1</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1179,11 +1287,17 @@
       <c r="D20" s="13">
         <v>1</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="13"/>
+      <c r="H20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1199,11 +1313,17 @@
       <c r="D21" s="13">
         <v>1</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="13"/>
+      <c r="H21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1219,11 +1339,17 @@
       <c r="D22" s="13">
         <v>1</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="13"/>
+      <c r="H22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1239,11 +1365,17 @@
       <c r="D23" s="13">
         <v>1</v>
       </c>
-      <c r="E23" s="13"/>
+      <c r="E23" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="13"/>
+      <c r="H23" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1262,12 +1394,10 @@
       <c r="E24" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>75</v>
-      </c>
+      <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>74</v>
@@ -1293,7 +1423,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>74</v>
@@ -1314,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="E26" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="G26" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H26" s="9" t="b">
         <v>1</v>
@@ -1328,7 +1458,9 @@
       <c r="I26" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="10"/>
+      <c r="J26" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -1344,13 +1476,13 @@
         <v>5</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H27" s="9" t="b">
         <v>1</v>
@@ -1359,7 +1491,7 @@
         <v>74</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1381,7 +1513,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>74</v>
@@ -1407,7 +1539,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>74</v>
@@ -1428,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H30" s="9" t="b">
         <v>1</v>
@@ -1443,7 +1575,7 @@
         <v>74</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1460,13 +1592,13 @@
         <v>9</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H31" s="9" t="b">
         <v>1</v>
@@ -1475,7 +1607,7 @@
         <v>74</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1497,7 +1629,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>74</v>
@@ -1518,13 +1650,13 @@
         <v>11</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H33" s="9" t="b">
         <v>1</v>
@@ -1533,7 +1665,7 @@
         <v>74</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1595,7 +1727,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>74</v>
@@ -1621,7 +1753,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>74</v>
@@ -1647,7 +1779,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>74</v>
@@ -1673,7 +1805,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I39" s="13" t="s">
         <v>74</v>
@@ -1699,7 +1831,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>74</v>
@@ -1725,7 +1857,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I41" s="13" t="s">
         <v>74</v>
@@ -1751,7 +1883,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I42" s="13" t="s">
         <v>74</v>
@@ -1777,7 +1909,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I43" s="13" t="s">
         <v>74</v>
@@ -1798,13 +1930,13 @@
         <v>19</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H44" s="9" t="b">
         <v>1</v>
@@ -1813,7 +1945,7 @@
         <v>74</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1835,7 +1967,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>74</v>
@@ -1861,7 +1993,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I46" s="13" t="s">
         <v>74</v>
@@ -1887,7 +2019,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I47" s="13" t="s">
         <v>74</v>
@@ -1913,7 +2045,7 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I48" s="13" t="s">
         <v>74</v>
@@ -1939,7 +2071,7 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>74</v>
@@ -1965,7 +2097,7 @@
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>74</v>
@@ -1991,7 +2123,7 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>74</v>
@@ -2017,7 +2149,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>74</v>
@@ -2043,7 +2175,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>74</v>
@@ -2069,7 +2201,7 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I54" s="13" t="s">
         <v>74</v>
@@ -2095,7 +2227,7 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I55" s="13" t="s">
         <v>74</v>
@@ -2121,7 +2253,7 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I56" s="13" t="s">
         <v>74</v>
@@ -2147,7 +2279,7 @@
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
       <c r="H57" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I57" s="13" t="s">
         <v>74</v>
@@ -2173,7 +2305,7 @@
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>74</v>
@@ -2199,7 +2331,7 @@
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I59" s="13" t="s">
         <v>74</v>
@@ -2225,7 +2357,7 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>74</v>
@@ -2240,7 +2372,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D61" s="13">
         <v>36</v>
@@ -2251,7 +2383,7 @@
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I61" s="13" t="s">
         <v>74</v>
@@ -2277,7 +2409,7 @@
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>74</v>
@@ -2298,13 +2430,13 @@
         <v>38</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H63" s="9" t="b">
         <v>1</v>
@@ -2313,7 +2445,7 @@
         <v>74</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds new (Z)ombie feature. Also adds new test case and results as well as 6.0 section to the test plan.
</commit_message>
<xml_diff>
--- a/docs/assignmnet7/Requirments_Matrix.xlsx
+++ b/docs/assignmnet7/Requirments_Matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="10335"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="109">
   <si>
     <t>Operate as a console application</t>
   </si>
@@ -337,16 +337,22 @@
   </si>
   <si>
     <t>Blank line is now ignored</t>
+  </si>
+  <si>
+    <t>Zombie image will be invoked by 'Z'.  This will display an ascii image of a zombie.</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -402,12 +408,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -451,6 +470,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,7 +576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -576,7 +610,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -752,17 +785,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="24.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.28515625" style="11" bestFit="1" customWidth="1"/>
@@ -774,7 +807,7 @@
     <col min="10" max="10" width="35.140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="37.5">
       <c r="A1" s="5" t="s">
         <v>91</v>
       </c>
@@ -806,7 +839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -832,7 +865,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -858,7 +891,7 @@
       </c>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -884,7 +917,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -910,7 +943,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -936,7 +969,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3">
         <v>4.2</v>
       </c>
@@ -962,7 +995,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="3">
         <v>4.2</v>
       </c>
@@ -988,7 +1021,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="3">
         <v>4.2</v>
       </c>
@@ -1014,7 +1047,7 @@
       </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="3">
         <v>4.2</v>
       </c>
@@ -1040,7 +1073,7 @@
       </c>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="3">
         <v>4.2</v>
       </c>
@@ -1066,7 +1099,7 @@
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="3">
         <v>4.2</v>
       </c>
@@ -1092,7 +1125,7 @@
       </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="3">
         <v>4.2</v>
       </c>
@@ -1118,7 +1151,7 @@
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="3">
         <v>4.2</v>
       </c>
@@ -1144,7 +1177,7 @@
       </c>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="3">
         <v>4.2</v>
       </c>
@@ -1170,7 +1203,7 @@
       </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30">
       <c r="A16" s="3">
         <v>4.2</v>
       </c>
@@ -1196,7 +1229,7 @@
       </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="3">
         <v>4.2</v>
       </c>
@@ -1222,7 +1255,7 @@
       </c>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="75">
       <c r="A18" s="3">
         <v>4.2</v>
       </c>
@@ -1248,7 +1281,7 @@
       </c>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="45">
       <c r="A19" s="3">
         <v>4.2</v>
       </c>
@@ -1274,7 +1307,7 @@
       </c>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="45">
       <c r="A20" s="3">
         <v>4.2</v>
       </c>
@@ -1300,7 +1333,7 @@
       </c>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="75">
       <c r="A21" s="3">
         <v>4.2</v>
       </c>
@@ -1326,7 +1359,7 @@
       </c>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="30">
       <c r="A22" s="3">
         <v>4.2</v>
       </c>
@@ -1352,7 +1385,7 @@
       </c>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="45">
       <c r="A23" s="3">
         <v>4.2</v>
       </c>
@@ -1378,7 +1411,7 @@
       </c>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="30">
       <c r="A24" s="3">
         <v>4.3</v>
       </c>
@@ -1404,7 +1437,7 @@
       </c>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="30">
       <c r="A25" s="3">
         <v>4.3</v>
       </c>
@@ -1430,7 +1463,7 @@
       </c>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="45">
       <c r="A26" s="3">
         <v>4.3</v>
       </c>
@@ -1462,7 +1495,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="45">
       <c r="A27" s="3">
         <v>4.3</v>
       </c>
@@ -1494,7 +1527,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30">
       <c r="A28" s="3">
         <v>4.3</v>
       </c>
@@ -1520,7 +1553,7 @@
       </c>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="3">
         <v>4.3</v>
       </c>
@@ -1546,7 +1579,7 @@
       </c>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="45">
       <c r="A30" s="3">
         <v>4.3</v>
       </c>
@@ -1578,7 +1611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="45">
       <c r="A31" s="3">
         <v>4.3</v>
       </c>
@@ -1610,7 +1643,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="45">
       <c r="A32" s="3">
         <v>4.3</v>
       </c>
@@ -1636,7 +1669,7 @@
       </c>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="60">
       <c r="A33" s="3">
         <v>4.3</v>
       </c>
@@ -1668,7 +1701,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="45">
       <c r="A34" s="3">
         <v>5</v>
       </c>
@@ -1688,7 +1721,7 @@
       <c r="I34" s="13"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="4" t="s">
         <v>25</v>
       </c>
@@ -1708,7 +1741,7 @@
       <c r="I35" s="13"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
@@ -1734,7 +1767,7 @@
       </c>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
@@ -1760,7 +1793,7 @@
       </c>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="30">
       <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
@@ -1786,7 +1819,7 @@
       </c>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
         <v>25</v>
       </c>
@@ -1812,7 +1845,7 @@
       </c>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="45">
       <c r="A40" s="4" t="s">
         <v>25</v>
       </c>
@@ -1838,7 +1871,7 @@
       </c>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="30">
       <c r="A41" s="3">
         <v>5.2</v>
       </c>
@@ -1864,7 +1897,7 @@
       </c>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="45">
       <c r="A42" s="2">
         <v>5.2</v>
       </c>
@@ -1890,7 +1923,7 @@
       </c>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="30">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1916,7 +1949,7 @@
       </c>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="45">
       <c r="A44" s="4" t="s">
         <v>29</v>
       </c>
@@ -1948,7 +1981,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="60">
       <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
@@ -1974,7 +2007,7 @@
       </c>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="45">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
@@ -2000,7 +2033,7 @@
       </c>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="30">
       <c r="A47" s="4" t="s">
         <v>32</v>
       </c>
@@ -2026,7 +2059,7 @@
       </c>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
         <v>36</v>
       </c>
@@ -2052,7 +2085,7 @@
       </c>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="45">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
@@ -2078,7 +2111,7 @@
       </c>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="30">
       <c r="A50" s="4" t="s">
         <v>36</v>
       </c>
@@ -2104,7 +2137,7 @@
       </c>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="30">
       <c r="A51" s="4" t="s">
         <v>37</v>
       </c>
@@ -2130,7 +2163,7 @@
       </c>
       <c r="J51" s="10"/>
     </row>
-    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="45">
       <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
@@ -2156,7 +2189,7 @@
       </c>
       <c r="J52" s="10"/>
     </row>
-    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="30">
       <c r="A53" s="4" t="s">
         <v>38</v>
       </c>
@@ -2182,7 +2215,7 @@
       </c>
       <c r="J53" s="10"/>
     </row>
-    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="45">
       <c r="A54" s="4" t="s">
         <v>38</v>
       </c>
@@ -2208,7 +2241,7 @@
       </c>
       <c r="J54" s="10"/>
     </row>
-    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="45">
       <c r="A55" s="4" t="s">
         <v>46</v>
       </c>
@@ -2234,7 +2267,7 @@
       </c>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="30">
       <c r="A56" s="4" t="s">
         <v>46</v>
       </c>
@@ -2260,7 +2293,7 @@
       </c>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="45">
       <c r="A57" s="4" t="s">
         <v>46</v>
       </c>
@@ -2286,7 +2319,7 @@
       </c>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="45">
       <c r="A58" s="4" t="s">
         <v>47</v>
       </c>
@@ -2312,7 +2345,7 @@
       </c>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="30">
       <c r="A59" s="4" t="s">
         <v>47</v>
       </c>
@@ -2338,7 +2371,7 @@
       </c>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="60">
       <c r="A60" s="4" t="s">
         <v>49</v>
       </c>
@@ -2364,7 +2397,7 @@
       </c>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="75">
       <c r="A61" s="4" t="s">
         <v>49</v>
       </c>
@@ -2390,7 +2423,7 @@
       </c>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="60">
       <c r="A62" s="4" t="s">
         <v>50</v>
       </c>
@@ -2416,37 +2449,63 @@
       </c>
       <c r="J62" s="10"/>
     </row>
-    <row r="63" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+    <row r="63" spans="1:10" ht="60">
+      <c r="A63" s="15">
         <v>5.3</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="15">
         <v>62</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D63" s="17">
         <v>38</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="H63" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="J63" s="10" t="s">
+      <c r="H63" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J63" s="16" t="s">
         <v>94</v>
       </c>
+    </row>
+    <row r="64" spans="1:10" s="20" customFormat="1" ht="30">
+      <c r="A64" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="B64" s="2">
+        <v>63</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="13">
+        <v>39</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J64" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2464,24 +2523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>